<commit_message>
23/05/2018 - Cotação atualizada
</commit_message>
<xml_diff>
--- a/Controle BTC.xlsx
+++ b/Controle BTC.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="101">
   <si>
     <t>Tipo</t>
   </si>
@@ -2115,11 +2115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-212656768"/>
-        <c:axId val="-212656224"/>
+        <c:axId val="147073696"/>
+        <c:axId val="147080768"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-212656768"/>
+        <c:axId val="147073696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,14 +2161,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-212656224"/>
+        <c:crossAx val="147080768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-212656224"/>
+        <c:axId val="147080768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2218,7 +2218,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-212656768"/>
+        <c:crossAx val="147073696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2293,6 +2293,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2503,11 +2504,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194215520"/>
-        <c:axId val="-194220416"/>
+        <c:axId val="381470992"/>
+        <c:axId val="381481872"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194215520"/>
+        <c:axId val="381470992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2550,14 +2551,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194220416"/>
+        <c:crossAx val="381481872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194220416"/>
+        <c:axId val="381481872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2608,7 +2609,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194215520"/>
+        <c:crossAx val="381470992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2672,6 +2673,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2882,11 +2884,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176717056"/>
-        <c:axId val="-176717600"/>
+        <c:axId val="381469360"/>
+        <c:axId val="381482960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-176717056"/>
+        <c:axId val="381469360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2929,14 +2931,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176717600"/>
+        <c:crossAx val="381482960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-176717600"/>
+        <c:axId val="381482960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2987,7 +2989,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176717056"/>
+        <c:crossAx val="381469360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3304,11 +3306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176712704"/>
-        <c:axId val="-176718688"/>
+        <c:axId val="381468816"/>
+        <c:axId val="381475344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-176712704"/>
+        <c:axId val="381468816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3351,14 +3353,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176718688"/>
+        <c:crossAx val="381475344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-176718688"/>
+        <c:axId val="381475344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3409,7 +3411,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176712704"/>
+        <c:crossAx val="381468816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3550,7 +3552,7 @@
                   <c:v>0.24225165700000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.35326293500000006</c:v>
+                  <c:v>0.35253405300000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3650,7 +3652,7 @@
                   <c:v>0.859536144</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3114086299999999</c:v>
+                  <c:v>1.30900931</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3687,11 +3689,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176714336"/>
-        <c:axId val="-176713248"/>
+        <c:axId val="381480240"/>
+        <c:axId val="381478608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-176714336"/>
+        <c:axId val="381480240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3734,7 +3736,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176713248"/>
+        <c:crossAx val="381478608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3742,7 +3744,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-176713248"/>
+        <c:axId val="381478608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3793,7 +3795,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176714336"/>
+        <c:crossAx val="381480240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4110,11 +4112,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176716512"/>
-        <c:axId val="-176713792"/>
+        <c:axId val="381479152"/>
+        <c:axId val="381480784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-176716512"/>
+        <c:axId val="381479152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4157,14 +4159,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176713792"/>
+        <c:crossAx val="381480784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-176713792"/>
+        <c:axId val="381480784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4215,7 +4217,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176716512"/>
+        <c:crossAx val="381479152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4550,11 +4552,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176715968"/>
-        <c:axId val="-176715424"/>
+        <c:axId val="381482416"/>
+        <c:axId val="381481328"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-176715968"/>
+        <c:axId val="381482416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4597,14 +4599,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176715424"/>
+        <c:crossAx val="381481328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-176715424"/>
+        <c:axId val="381481328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4655,7 +4657,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176715968"/>
+        <c:crossAx val="381482416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4990,11 +4992,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-176712160"/>
-        <c:axId val="-176711616"/>
+        <c:axId val="381473712"/>
+        <c:axId val="381473168"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-176712160"/>
+        <c:axId val="381473712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5037,14 +5039,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176711616"/>
+        <c:crossAx val="381473168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-176711616"/>
+        <c:axId val="381473168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5095,7 +5097,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-176712160"/>
+        <c:crossAx val="381473712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5190,6 +5192,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5472,11 +5475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-212655680"/>
-        <c:axId val="-409367600"/>
+        <c:axId val="147074240"/>
+        <c:axId val="147074784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-212655680"/>
+        <c:axId val="147074240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5518,14 +5521,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-409367600"/>
+        <c:crossAx val="147074784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-409367600"/>
+        <c:axId val="147074784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5575,7 +5578,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-212655680"/>
+        <c:crossAx val="147074240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5690,6 +5693,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5912,11 +5916,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-409357808"/>
-        <c:axId val="-410234368"/>
+        <c:axId val="147075328"/>
+        <c:axId val="147075872"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-409357808"/>
+        <c:axId val="147075328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5958,14 +5962,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-410234368"/>
+        <c:crossAx val="147075872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-410234368"/>
+        <c:axId val="147075872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6015,7 +6019,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-409357808"/>
+        <c:crossAx val="147075328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6090,6 +6094,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6165,10 +6170,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Total!$H$20:$H$46</c:f>
+              <c:f>Total!$H$20:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43215</c:v>
                 </c:pt>
@@ -6249,18 +6254,24 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43241</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$L$20:$L$46</c:f>
+              <c:f>Total!$L$20:$L$48</c:f>
               <c:numCache>
                 <c:formatCode>"R$"#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>58.612591555555554</c:v>
+                  <c:v>58.613854000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>126.75359499999999</c:v>
@@ -6339,6 +6350,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>202.58713399999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>206.80042099999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>201.22851739999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6354,11 +6371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194219872"/>
-        <c:axId val="-194220960"/>
+        <c:axId val="147078592"/>
+        <c:axId val="147079136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194219872"/>
+        <c:axId val="147078592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6400,14 +6417,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194220960"/>
+        <c:crossAx val="147079136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194220960"/>
+        <c:axId val="147079136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6457,7 +6474,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194219872"/>
+        <c:crossAx val="147078592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6532,6 +6549,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6607,10 +6625,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Cotação!$A$3:$A$29</c:f>
+              <c:f>Cotação!$A$3:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43216</c:v>
                 </c:pt>
@@ -6691,16 +6709,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Cotação!$D$3:$D$29</c:f>
+              <c:f>Cotação!$D$3:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>"R$"#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>32640</c:v>
                 </c:pt>
@@ -6781,6 +6802,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>30448</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6796,11 +6820,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194217152"/>
-        <c:axId val="-194222048"/>
+        <c:axId val="147081856"/>
+        <c:axId val="147082400"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194217152"/>
+        <c:axId val="147081856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6842,14 +6866,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194222048"/>
+        <c:crossAx val="147082400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194222048"/>
+        <c:axId val="147082400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6899,7 +6923,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194217152"/>
+        <c:crossAx val="147081856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6974,6 +6998,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7049,10 +7074,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Cotação!$A$3:$A$29</c:f>
+              <c:f>Cotação!$A$3:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43216</c:v>
                 </c:pt>
@@ -7133,16 +7158,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Cotação!$F$3:$F$29</c:f>
+              <c:f>Cotação!$F$3:$F$30</c:f>
               <c:numCache>
                 <c:formatCode>"R$"#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>3.4754999999999998</c:v>
                 </c:pt>
@@ -7223,6 +7251,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>3.6471</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.6284999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7238,11 +7269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194218240"/>
-        <c:axId val="-194222592"/>
+        <c:axId val="147083488"/>
+        <c:axId val="147084032"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194218240"/>
+        <c:axId val="147083488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7284,14 +7315,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194222592"/>
+        <c:crossAx val="147084032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194222592"/>
+        <c:axId val="147084032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7341,7 +7372,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194218240"/>
+        <c:crossAx val="147083488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7416,6 +7447,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7491,10 +7523,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Cotação!$A$3:$A$29</c:f>
+              <c:f>Cotação!$A$3:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>43216</c:v>
                 </c:pt>
@@ -7575,16 +7607,19 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Cotação!$B$3:$B$29</c:f>
+              <c:f>Cotação!$B$3:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>[$$-409]#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>9279.2999999999993</c:v>
                 </c:pt>
@@ -7665,6 +7700,9 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>8057.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7584.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7680,11 +7718,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194219328"/>
-        <c:axId val="-194221504"/>
+        <c:axId val="146106176"/>
+        <c:axId val="146113248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194219328"/>
+        <c:axId val="146106176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7726,14 +7764,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194221504"/>
+        <c:crossAx val="146113248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194221504"/>
+        <c:axId val="146113248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7783,7 +7821,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194219328"/>
+        <c:crossAx val="146106176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7921,10 +7959,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Total!$H$20:$H$46</c:f>
+              <c:f>Total!$H$20:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43215</c:v>
                 </c:pt>
@@ -8005,18 +8043,24 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43241</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$L$20:$L$46</c:f>
+              <c:f>Total!$L$20:$L$48</c:f>
               <c:numCache>
                 <c:formatCode>"R$"#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>58.612591555555554</c:v>
+                  <c:v>58.613854000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>126.75359499999999</c:v>
@@ -8095,6 +8139,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>202.58713399999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>206.80042099999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>201.22851739999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8110,11 +8160,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-194217696"/>
-        <c:axId val="-194218784"/>
+        <c:axId val="146118144"/>
+        <c:axId val="146109984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194217696"/>
+        <c:axId val="146118144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8157,14 +8207,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194218784"/>
+        <c:crossAx val="146109984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194218784"/>
+        <c:axId val="146109984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8215,7 +8265,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194217696"/>
+        <c:crossAx val="146118144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8354,10 +8404,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Total!$H$20:$H$46</c:f>
+              <c:f>Total!$H$20:$H$48</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>43215</c:v>
                 </c:pt>
@@ -8438,21 +8488,27 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>43241</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>43242</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$M$20:$M$46</c:f>
+              <c:f>Total!$M$20:$M$48</c:f>
               <c:numCache>
                 <c:formatCode>"R$"#,##0.00</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.141003444444436</c:v>
+                  <c:v>68.139740999999987</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.1866181360000212</c:v>
@@ -8528,6 +8584,12 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-0.48914800000000014</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.2132869999999798</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-5.5719035999999846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8544,11 +8606,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-194216608"/>
-        <c:axId val="-194216064"/>
+        <c:axId val="381470448"/>
+        <c:axId val="381476432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-194216608"/>
+        <c:axId val="381470448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8591,14 +8653,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194216064"/>
+        <c:crossAx val="381476432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-194216064"/>
+        <c:axId val="381476432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8649,7 +8711,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-194216608"/>
+        <c:crossAx val="381470448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17985,8 +18047,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela25" displayName="Tabela25" ref="A2:G29" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
-  <autoFilter ref="A2:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela25" displayName="Tabela25" ref="A2:G30" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="A2:G30"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Data" dataDxfId="48"/>
     <tableColumn id="2" name="BTC/USD" dataDxfId="47"/>
@@ -18007,8 +18069,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="H19:N46" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
-  <autoFilter ref="H19:N46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="H19:N48" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+  <autoFilter ref="H19:N48"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Data" dataDxfId="39"/>
     <tableColumn id="2" name="Atlas" dataDxfId="38">
@@ -18600,7 +18662,7 @@
       <c r="Q1" s="121"/>
       <c r="R1" s="120">
         <f>SUM(Atlas!A7,AWS!K1,Easy!L22)</f>
-        <v>204.45195708</v>
+        <v>201.22851739999999</v>
       </c>
       <c r="S1" s="120"/>
       <c r="T1" s="120"/>
@@ -18642,7 +18704,7 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18720,7 +18782,7 @@
       </c>
       <c r="J2" s="38">
         <f>AVERAGE(Tabela25[USD/BRL])</f>
-        <v>3.5864185185185189</v>
+        <v>3.5879214285714291</v>
       </c>
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
@@ -18771,7 +18833,7 @@
       </c>
       <c r="J3" s="117">
         <f>AVERAGE(Tabela25[BTC/BRL])</f>
-        <v>32448.751851851852</v>
+        <v>32321.653571428575</v>
       </c>
       <c r="L3" s="27"/>
       <c r="M3" s="27"/>
@@ -18822,7 +18884,7 @@
       </c>
       <c r="J4" s="118">
         <f>AVERAGE(Tabela25[BTC/USD])</f>
-        <v>8911.4518518518507</v>
+        <v>8864.0499999999993</v>
       </c>
       <c r="L4" s="27"/>
       <c r="M4" s="27"/>
@@ -19255,7 +19317,7 @@
       </c>
       <c r="J13" s="117">
         <f>SMALL(Tabela25[BTC/BRL],1)</f>
-        <v>30383</v>
+        <v>28890</v>
       </c>
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
@@ -19305,7 +19367,7 @@
       </c>
       <c r="J14" s="118">
         <f>SMALL(Tabela25[BTC/USD],1)</f>
-        <v>8001.4</v>
+        <v>7584.2</v>
       </c>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
@@ -19982,6 +20044,30 @@
       <c r="AB29" s="27"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>43243</v>
+      </c>
+      <c r="B30" s="4">
+        <v>7584.2</v>
+      </c>
+      <c r="C30" s="4" t="str">
+        <f>IF(Tabela25[[#This Row],[BTC/USD]]&lt;B29,"▼",IF(Tabela25[[#This Row],[BTC/USD]]&gt;B29,"▲","-"))</f>
+        <v>▼</v>
+      </c>
+      <c r="D30" s="5">
+        <v>28890</v>
+      </c>
+      <c r="E30" s="5" t="str">
+        <f>IF(Tabela25[[#This Row],[BTC/BRL]]&lt;D29,"▼",IF(Tabela25[[#This Row],[BTC/BRL]]&gt;D29,"▲","-"))</f>
+        <v>▼</v>
+      </c>
+      <c r="F30" s="5">
+        <v>3.6284999999999998</v>
+      </c>
+      <c r="G30" s="5" t="str">
+        <f>IF(Tabela25[[#This Row],[USD/BRL]]&lt;F29,"▼",IF(Tabela25[[#This Row],[USD/BRL]]&gt;F29,"▲","-"))</f>
+        <v>▼</v>
+      </c>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
@@ -20103,10 +20189,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A18:R46"/>
+  <dimension ref="A18:R48"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20162,7 +20248,7 @@
       </c>
       <c r="J20" s="5">
         <f>IFERROR(VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela3[[Data]:[Saldo BRL]],5),0)</f>
-        <v>3.0125915555555558</v>
+        <v>3.0138540000000003</v>
       </c>
       <c r="K20" s="5">
         <f>VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela16[#All],3)</f>
@@ -20170,7 +20256,7 @@
       </c>
       <c r="L20" s="5">
         <f>SUM(Tabela6[[#This Row],[Atlas]:[Easy]])</f>
-        <v>58.612591555555554</v>
+        <v>58.613854000000003</v>
       </c>
       <c r="M20" s="5">
         <f>IFERROR(Tabela6[[#This Row],[Total]]-L19,0)</f>
@@ -20209,19 +20295,19 @@
       </c>
       <c r="M21" s="5">
         <f>IFERROR(Tabela6[[#This Row],[Total]]-L20,0)</f>
-        <v>68.141003444444436</v>
+        <v>68.139740999999987</v>
       </c>
       <c r="N21" s="3">
         <f>Tabela6[[#This Row],[Variação]]/Tabela6[[#This Row],[Total]]</f>
-        <v>0.53758635756598805</v>
+        <v>0.53757639773451782</v>
       </c>
       <c r="Q21" s="99">
         <f>AVERAGE(Tabela6[Variação %])</f>
-        <v>3.7040306533704173E-2</v>
+        <v>3.4233192072230252E-2</v>
       </c>
       <c r="R21" s="71">
         <f>AVERAGE(Tabela6[Variação])</f>
-        <v>5.3323904609053496</v>
+        <v>4.917747013793103</v>
       </c>
     </row>
     <row r="22" spans="8:18" x14ac:dyDescent="0.25">
@@ -20947,6 +21033,64 @@
       <c r="N46" s="3">
         <f>Tabela6[[#This Row],[Variação]]/Tabela6[[#This Row],[Total]]</f>
         <v>-2.4145067376292522E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H47" s="90">
+        <v>43242</v>
+      </c>
+      <c r="I47" s="5">
+        <f>IFERROR(VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela1[[Data ]:[BRL]],9),0)</f>
+        <v>65.344158000000007</v>
+      </c>
+      <c r="J47" s="5">
+        <f>IFERROR(VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela3[[Data]:[Saldo BRL]],5),0)</f>
+        <v>85.816262999999992</v>
+      </c>
+      <c r="K47" s="5">
+        <f>VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela16[#All],3)</f>
+        <v>55.64</v>
+      </c>
+      <c r="L47" s="5">
+        <f>SUM(Tabela6[[#This Row],[Atlas]:[Easy]])</f>
+        <v>206.80042099999997</v>
+      </c>
+      <c r="M47" s="5">
+        <f>IFERROR(Tabela6[[#This Row],[Total]]-L46,0)</f>
+        <v>4.2132869999999798</v>
+      </c>
+      <c r="N47" s="3">
+        <f>Tabela6[[#This Row],[Variação]]/Tabela6[[#This Row],[Total]]</f>
+        <v>2.0373686763432559E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H48" s="90">
+        <v>43243</v>
+      </c>
+      <c r="I48" s="5">
+        <f>IFERROR(VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela1[[Data ]:[BRL]],9),0)</f>
+        <v>59.772254399999994</v>
+      </c>
+      <c r="J48" s="5">
+        <f>IFERROR(VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela3[[Data]:[Saldo BRL]],5),0)</f>
+        <v>85.816262999999992</v>
+      </c>
+      <c r="K48" s="5">
+        <f>VLOOKUP(Tabela6[[#This Row],[Data]]+1,Tabela16[#All],3)</f>
+        <v>55.64</v>
+      </c>
+      <c r="L48" s="5">
+        <f>SUM(Tabela6[[#This Row],[Atlas]:[Easy]])</f>
+        <v>201.22851739999999</v>
+      </c>
+      <c r="M48" s="5">
+        <f>IFERROR(Tabela6[[#This Row],[Total]]-L47,0)</f>
+        <v>-5.5719035999999846</v>
+      </c>
+      <c r="N48" s="3">
+        <f>Tabela6[[#This Row],[Variação]]/Tabela6[[#This Row],[Total]]</f>
+        <v>-2.7689433247297706E-2</v>
       </c>
     </row>
   </sheetData>
@@ -21688,8 +21832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21906,11 +22050,11 @@
       </c>
       <c r="J6" s="43">
         <f>IF((SUMIFS(Tabela1[Bruto USD],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))=0,"SR",SUMIFS(Tabela1[Bruto USD],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))</f>
-        <v>0.35326293500000006</v>
+        <v>0.35253405300000001</v>
       </c>
       <c r="K6" s="38">
         <f>IF((SUMIFS(Tabela1[Bruto BRL],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))=0,"SR",SUMIFS(Tabela1[Bruto BRL],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))</f>
-        <v>1.3114086299999999</v>
+        <v>1.30900931</v>
       </c>
       <c r="L6" s="39">
         <f>IF((SUMIFS(Tabela1[porcentagem],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))=0,"SR",SUMIFS(Tabela1[porcentagem],Tabela1[Mês],Plan4!A5,Tabela1[Ano],L$1))</f>
@@ -21929,7 +22073,7 @@
     <row r="7" spans="1:22" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="141">
         <f>INDEX(Tabela1[BRL],MATCH(9.99999999999999+307,Tabela1[BRL]))</f>
-        <v>62.99569408</v>
+        <v>59.772254399999994</v>
       </c>
       <c r="B7" s="141"/>
       <c r="C7" s="141"/>
@@ -21941,7 +22085,7 @@
       </c>
       <c r="G7" s="61">
         <f>AVERAGE(Tabela1[Bruto BRL])</f>
-        <v>8.349787592307692E-2</v>
+        <v>8.3405594384615395E-2</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="20" t="s">
@@ -22060,7 +22204,7 @@
       </c>
       <c r="G10" s="67">
         <f>SMALL(Tabela1[USD],1)</f>
-        <v>16.467361283999999</v>
+        <v>15.691406431999999</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="21" t="s">
@@ -22097,7 +22241,7 @@
       <c r="C11" s="149"/>
       <c r="D11" s="148">
         <f>SUM(Tabela1[Bruto BRL])</f>
-        <v>2.1709447740000001</v>
+        <v>2.1685454540000002</v>
       </c>
       <c r="E11" s="148"/>
       <c r="F11" s="68">
@@ -23754,19 +23898,19 @@
       </c>
       <c r="H59" s="72">
         <f>Tabela1[[#This Row],[Posterior]]*VLOOKUP(Tabela1[[#This Row],[Data ]],Tabela25[],2)</f>
-        <v>16.670645199999999</v>
+        <v>15.691406431999999</v>
       </c>
       <c r="I59" s="73">
         <f>Tabela1[[#This Row],[Posterior]]*VLOOKUP(Tabela1[[#This Row],[Data ]],Tabela25[],4)</f>
-        <v>62.99569408</v>
+        <v>59.772254399999994</v>
       </c>
       <c r="J59" s="73">
         <f>IF(Tabela1[[#This Row],[Tipo]]="Depósito (BTC)","N/A",Tabela1[[#This Row],[Variação]]*VLOOKUP(Tabela1[[#This Row],[Data ]],Tabela25[],4))</f>
-        <v>4.6889920000000002E-2</v>
+        <v>4.4490600000000005E-2</v>
       </c>
       <c r="K59" s="74">
         <f>IF(Tabela1[[#This Row],[Tipo]]="Depósito (BTC)","N/A",Tabela1[[#This Row],[Variação]]*VLOOKUP(Tabela1[[#This Row],[Data ]],Tabela25[],2))</f>
-        <v>1.2408550000000001E-2</v>
+        <v>1.1679668000000001E-2</v>
       </c>
       <c r="L59" s="75">
         <f>G59/E59</f>
@@ -23823,8 +23967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23918,7 +24062,7 @@
       </c>
       <c r="K6" s="95">
         <f ca="1">J6*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>3.063564</v>
+        <v>3.0479399999999996</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -23931,7 +24075,7 @@
       </c>
       <c r="K7" s="96">
         <f ca="1">J7*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>2.8605420999999995</v>
+        <v>2.8459534999999994</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -23944,7 +24088,7 @@
       </c>
       <c r="K8" s="96">
         <f ca="1">J8*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>85.816262999999992</v>
+        <v>85.378604999999993</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -23957,7 +24101,7 @@
       </c>
       <c r="K9" s="96">
         <f ca="1">J9*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>1029.7951559999999</v>
+        <v>1024.5432599999997</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -23970,7 +24114,7 @@
       </c>
       <c r="K10" s="96">
         <f ca="1">J10*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>3.1365059999999998</v>
+        <v>3.1205099999999999</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24005,7 +24149,7 @@
       </c>
       <c r="K13" s="95">
         <f ca="1">J13*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>145.88400000000001</v>
+        <v>145.13999999999999</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -24018,7 +24162,7 @@
       </c>
       <c r="K14" s="96">
         <f ca="1">J14*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>583.53600000000006</v>
+        <v>580.55999999999995</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24031,7 +24175,7 @@
       </c>
       <c r="K15" s="97">
         <f ca="1">J15*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>85.816262999999992</v>
+        <v>85.378604999999993</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -24044,7 +24188,7 @@
       </c>
       <c r="K16" s="113">
         <f ca="1">J16*VLOOKUP(TODAY(),Tabela25[],6)</f>
-        <v>-497.71973700000001</v>
+        <v>-495.18139499999995</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -24085,7 +24229,7 @@
       </c>
       <c r="E21" s="13">
         <f>IFERROR(Tabela3[[#This Row],[Saldo disponível para saque]]*VLOOKUP(Tabela3[[#This Row],[Data]],Tabela25[],6),Tabela3[[#This Row],[Saldo disponível para saque]]*Cotação!J2)</f>
-        <v>3.0125915555555558</v>
+        <v>3.0138540000000003</v>
       </c>
       <c r="F21" s="93">
         <v>0.4</v>
@@ -24698,6 +24842,9 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
       </c>
       <c r="C45" s="11">
         <v>0</v>

</xml_diff>